<commit_message>
idk where this change comes from but its an excel table and idc
</commit_message>
<xml_diff>
--- a/misc_results/misc_main_scripts/Compare_CFs/rmse_cc_table_samples_0-4-60.xlsx
+++ b/misc_results/misc_main_scripts/Compare_CFs/rmse_cc_table_samples_0-4-60.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>rmse</t>
   </si>
@@ -39,7 +39,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -49,14 +49,18 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -74,10 +78,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>